<commit_message>
06/10/2023 * Addition of UT_5029 to characterise loop gain and impact of parameter A
</commit_message>
<xml_diff>
--- a/result/no_regression.xlsx
+++ b/result/no_regression.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
   <si>
     <t>Test result number</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Expertise MUX SQUID V(Phi)</t>
   </si>
   <si>
-    <t>DRE_DMX_UT_5023</t>
-  </si>
-  <si>
     <t>Test close loop MUX SQUID</t>
   </si>
   <si>
@@ -157,6 +154,18 @@
   </si>
   <si>
     <t>Characterisation MUX SQUID TF-2</t>
+  </si>
+  <si>
+    <t>DRE_DMX_UT_5029</t>
+  </si>
+  <si>
+    <t>Test of feedback algo, impact of A=0</t>
+  </si>
+  <si>
+    <t>DRE_DMX_UT_5023a</t>
+  </si>
+  <si>
+    <t>DRE_DMX_UT_5023b</t>
   </si>
 </sst>
 </file>
@@ -963,15 +972,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1224,18 +1233,21 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
         <v>34</v>
       </c>
-      <c r="B24" t="s">
-        <v>35</v>
+      <c r="C24" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -1243,10 +1255,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
@@ -1254,10 +1266,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
@@ -1265,10 +1277,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
@@ -1276,12 +1288,34 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
         <v>44</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>45</v>
       </c>
-      <c r="C29" t="s">
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
11/10/2023 * UT_5023c added for multi pulses simulation * UT_5023d added for multi pulses and auto-relock simulation
</commit_message>
<xml_diff>
--- a/result/no_regression.xlsx
+++ b/result/no_regression.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
   <si>
     <t>Test result number</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Expertise MUX SQUID V(Phi)</t>
   </si>
   <si>
-    <t>Test close loop MUX SQUID</t>
-  </si>
-  <si>
     <t>DRE_DMX_UT_5024</t>
   </si>
   <si>
@@ -166,6 +163,33 @@
   </si>
   <si>
     <t>DRE_DMX_UT_5023b</t>
+  </si>
+  <si>
+    <t>DRE_DMX_UT_5023c</t>
+  </si>
+  <si>
+    <t>Test close loop MUX SQUID (make pulse)</t>
+  </si>
+  <si>
+    <t>Test close loop MUX SQUID (make pulseS)</t>
+  </si>
+  <si>
+    <t>NOT PASS</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Some pixels didn't lock due to a pb in the dmx firmware (feedback integrator incorrectly initialized)</t>
+  </si>
+  <si>
+    <t>Flux jump due to a bad operating point</t>
+  </si>
+  <si>
+    <t>DRE_DMX_UT_5023d</t>
+  </si>
+  <si>
+    <t>Test close loop MUX SQUID (make pulseS and auto-relock)</t>
   </si>
 </sst>
 </file>
@@ -972,19 +996,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.42578125" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -994,8 +1019,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1006,7 +1034,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1017,7 +1045,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1028,7 +1056,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1039,7 +1067,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1050,7 +1078,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1061,7 +1089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1072,7 +1100,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1083,7 +1111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1094,7 +1122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1105,7 +1133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1116,7 +1144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1127,7 +1155,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1138,7 +1166,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1149,7 +1177,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1160,7 +1188,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1168,7 +1196,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1179,7 +1207,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1190,7 +1218,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1201,7 +1229,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1212,7 +1240,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1223,7 +1251,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1231,91 +1259,119 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>47</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>34</v>
       </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B28" t="s">
         <v>35</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>36</v>
       </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B29" t="s">
         <v>37</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>38</v>
       </c>
-      <c r="C27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B30" t="s">
         <v>39</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>40</v>
       </c>
-      <c r="C28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B31" t="s">
         <v>41</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>42</v>
       </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B32" t="s">
         <v>43</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>44</v>
       </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B33" t="s">
         <v>45</v>
       </c>
-      <c r="B31" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="C33" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
19/10/2023 * UT_5023x updated (closed loop simulations) * UT_5030x added (forward crosstalk simulations)
</commit_message>
<xml_diff>
--- a/result/no_regression.xlsx
+++ b/result/no_regression.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
   <si>
     <t>Test result number</t>
   </si>
@@ -190,6 +190,47 @@
   </si>
   <si>
     <t>Test close loop MUX SQUID (make pulseS and auto-relock)</t>
+  </si>
+  <si>
+    <t>DRE_DMX_UT_5030a</t>
+  </si>
+  <si>
+    <t>Crosstalk is observed</t>
+  </si>
+  <si>
+    <t>DRE_DMX_UT_5030b</t>
+  </si>
+  <si>
+    <t>DRE_DMX_UT_5030c</t>
+  </si>
+  <si>
+    <t>Simulation of forward crosstalk with pulse shaping=1
+and SAMPLING_DELAY=0x0008</t>
+  </si>
+  <si>
+    <t>Simulation of forward crosstalk with pulse shaping=1
+and SAMPLING_DELAY=x000B</t>
+  </si>
+  <si>
+    <t>Simulation of forward crosstalk with pulse shaping=1
+and SAMPLING_DELAY=0x0012</t>
+  </si>
+  <si>
+    <t>DRE_DMX_UT_5030d</t>
+  </si>
+  <si>
+    <t>Simulation of forward crosstalk with pulse shaping=3
+and SAMPLING_DELAY=0x0008</t>
+  </si>
+  <si>
+    <t>DRE_DMX_UT_5030e</t>
+  </si>
+  <si>
+    <t>Simulation of forward crosstalk with pulse shaping=3
+and SAMPLING_DELAY=0x000B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No crosstalk </t>
   </si>
 </sst>
 </file>
@@ -673,8 +714,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -996,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,7 +1408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -1373,6 +1417,76 @@
       </c>
       <c r="C33" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
15/12/2023 * Updates to characterise the delay correction between the Synchronisation and the pixels sequence
</commit_message>
<xml_diff>
--- a/result/no_regression.xlsx
+++ b/result/no_regression.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="89">
   <si>
     <t>Test result number</t>
   </si>
@@ -231,6 +231,66 @@
   </si>
   <si>
     <t xml:space="preserve">No crosstalk </t>
+  </si>
+  <si>
+    <t>DRE_DMX_UT_5031a</t>
+  </si>
+  <si>
+    <t>DRE_DMX_UT_5031b</t>
+  </si>
+  <si>
+    <t>DRE_DMX_UT_5031c</t>
+  </si>
+  <si>
+    <t>DRE_DMX_UT_5031d</t>
+  </si>
+  <si>
+    <t>DRE_DMX_UT_5031e</t>
+  </si>
+  <si>
+    <t>Simulation with g_RA_DELAY=0</t>
+  </si>
+  <si>
+    <t>Simulation with g_RA_DELAY=1</t>
+  </si>
+  <si>
+    <t>Simulation with g_RA_DELAY=2</t>
+  </si>
+  <si>
+    <t>Simulation with g_RA_DELAY=3</t>
+  </si>
+  <si>
+    <t>Simulation with g_RA_DELAY=4</t>
+  </si>
+  <si>
+    <t>RAS / DEMUX delay is not correct</t>
+  </si>
+  <si>
+    <t>DRE_DMX_UT_5031f</t>
+  </si>
+  <si>
+    <t>DRE_DMX_UT_5031g</t>
+  </si>
+  <si>
+    <t>Simulation with g_RA_DELAY=5</t>
+  </si>
+  <si>
+    <t>Simulation with g_RA_DELAY=6</t>
+  </si>
+  <si>
+    <t>DRE_DMX_UT_5032a</t>
+  </si>
+  <si>
+    <t>DRE_DMX_UT_5032b</t>
+  </si>
+  <si>
+    <t>RAS / DEMUX delay is correct</t>
+  </si>
+  <si>
+    <t>Simulation with g_RA_DELAY=6, g_ERROR_DELAY=0</t>
+  </si>
+  <si>
+    <t>Simulation with g_RA_DELAY=6, g_ERROR_DELAY=2</t>
   </si>
 </sst>
 </file>
@@ -1040,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37:D38"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,6 +1549,132 @@
         <v>58</v>
       </c>
     </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>